<commit_message>
Saving things for later.
</commit_message>
<xml_diff>
--- a/data/emergency.xlsx
+++ b/data/emergency.xlsx
@@ -14,13 +14,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fire Service Incidents
     </t>
   </si>
   <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>https://data.sa.gov.au/data/dataset/fire-service-incidents</t>
+  </si>
+  <si>
     <t>Category</t>
   </si>
   <si>
@@ -36,7 +39,13 @@
     <t xml:space="preserve">Drawn </t>
   </si>
   <si>
-    <t>https://data.sa.gov.au/data/dataset/fire-service-incidents</t>
+    <t>South Australian Metropolitan Fire Service</t>
+  </si>
+  <si>
+    <t>Historical Flood Mapping Proof of Concept</t>
+  </si>
+  <si>
+    <t>https://data.gov.au/dataset/535883f4-a038-49c0-bdac-cafb1ebb4836</t>
   </si>
   <si>
     <t>Uploaded</t>
@@ -48,22 +57,7 @@
     <t>Invasive species</t>
   </si>
   <si>
-    <t>Emergency</t>
-  </si>
-  <si>
-    <t>South Australian Metropolitan Fire Service</t>
-  </si>
-  <si>
-    <t>Historical Flood Mapping Proof of Concept</t>
-  </si>
-  <si>
-    <t>https://data.gov.au/dataset/535883f4-a038-49c0-bdac-cafb1ebb4836</t>
-  </si>
-  <si>
     <t>Geoscience Australia</t>
-  </si>
-  <si>
-    <t>The player you select loses 1 Flora or Fauna card each turn. Requires spending 2 facilities cards for them to clear.</t>
   </si>
   <si>
     <t xml:space="preserve">Indicators of Catchment Condition in the Intensive Land Use Zone of Australia – Feral animal density
@@ -76,6 +70,12 @@
     <t>Department of Agriculture</t>
   </si>
   <si>
+    <t>Emergency</t>
+  </si>
+  <si>
+    <t>A chosen player loses 1 Flora or Fauna each turn. 2 facilities cards needed to clear it. Card stays in front of selected player until cleared.</t>
+  </si>
+  <si>
     <t>Invasive species establishes itself in the spring.</t>
   </si>
   <si>
@@ -85,7 +85,7 @@
     <t>Bushfire</t>
   </si>
   <si>
-    <t>The player you select must discard all Flora cards, if they roll a 6 the plague affects you instead.</t>
+    <t>The player you select rolls 1 dice. Roll 1-5: they must discard all Flora cards. Roll 6: the plague affects you instead.</t>
   </si>
   <si>
     <t>You accidently initate a bushfire in a neighbouring park.</t>
@@ -97,7 +97,7 @@
     <t>Feral Animals</t>
   </si>
   <si>
-    <t>The player you select must discard all Fauna cards, if they roll a 6 the plague affects you instead.</t>
+    <t>The player you select rolls 1 dice. Roll 1-5: they must discard all Fauna cards. Roll 6: the plague affects you instead.</t>
   </si>
   <si>
     <t xml:space="preserve">A plague of feral animals kills all fauna in the park. </t>
@@ -133,10 +133,10 @@
     <t>Bushfire Disaster</t>
   </si>
   <si>
-    <t>State Emergency</t>
-  </si>
-  <si>
-    <t>All players (including yourself) loose all Flora cards.</t>
+    <t xml:space="preserve"> Emergency</t>
+  </si>
+  <si>
+    <t>State Emergency! All players (including yourself) lose all Flora cards.</t>
   </si>
   <si>
     <t>Extreme heatwave initates bushfires state wide.</t>
@@ -148,7 +148,7 @@
     <t>Lightning Storm</t>
   </si>
   <si>
-    <t>The player you select rolls 1 dice. Roll 1-3: they give that number of Fauna Cards to you. Roll 4-6: they keep their hand.</t>
+    <t>A selected player rolls 1 dice. Roll 1-3: they give that number of Fauna Cards to you. Roll 4-6: they keep their hand.</t>
   </si>
   <si>
     <t>A lightning storm runs through a park, scaring some Fauna away!</t>
@@ -182,20 +182,20 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <b/>
       <color rgb="FF000000"/>
     </font>
-    <font/>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
     <font>
       <sz val="10.0"/>
     </font>
     <font>
       <color rgb="FF000000"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
     </font>
     <font>
       <b/>
@@ -244,41 +244,41 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -313,36 +313,36 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -369,40 +369,40 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
+      <c r="F1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>10</v>
+      <c r="A2" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>20</v>
@@ -413,13 +413,13 @@
       <c r="F2" s="9"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -431,11 +431,11 @@
       <c r="F3" s="9"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>27</v>
@@ -453,7 +453,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>31</v>
@@ -471,7 +471,7 @@
         <v>34</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>35</v>
@@ -485,7 +485,7 @@
       <c r="F6" s="9"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -506,7 +506,7 @@
         <v>43</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>44</v>
@@ -520,14 +520,14 @@
       <c r="F8" s="9"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
+      <c r="A9" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>20</v>
@@ -538,11 +538,11 @@
       <c r="F9" s="9"/>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>27</v>
@@ -556,7 +556,7 @@
       <c r="F10" s="9"/>
     </row>
     <row r="18">
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -566,22 +566,22 @@
       </c>
     </row>
     <row r="22">
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="23">
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24">
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25">
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>